<commit_message>
Updated excel sheet and added attack stat
</commit_message>
<xml_diff>
--- a/JeremyItemInfo.xlsx
+++ b/JeremyItemInfo.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645"/>
   </bookViews>
   <sheets>
     <sheet name="DataLookUp" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="61" uniqueCount="38">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="212" uniqueCount="109">
   <si>
     <t>ID</t>
   </si>
@@ -118,22 +118,235 @@
     <t>EquipLoad?</t>
   </si>
   <si>
-    <t>EItemType!</t>
-  </si>
-  <si>
-    <t>EEquipmentType!</t>
-  </si>
-  <si>
-    <t>EItemRarity!</t>
-  </si>
-  <si>
-    <t>? = maybe not affect</t>
-  </si>
-  <si>
-    <t>! = chance of that variable occuring over another</t>
-  </si>
-  <si>
     <t>Note: there will be the need for rand float number from 0-1</t>
+  </si>
+  <si>
+    <t>EItemRarity</t>
+  </si>
+  <si>
+    <t>? = mayby does not need a formula</t>
+  </si>
+  <si>
+    <t>Potion of Healing</t>
+  </si>
+  <si>
+    <t>Lock Pick</t>
+  </si>
+  <si>
+    <t>Axe</t>
+  </si>
+  <si>
+    <t>Mace</t>
+  </si>
+  <si>
+    <t>Dagger</t>
+  </si>
+  <si>
+    <t>Arming Sword</t>
+  </si>
+  <si>
+    <t>Great Sword</t>
+  </si>
+  <si>
+    <t>Long Sword</t>
+  </si>
+  <si>
+    <t>Rapier</t>
+  </si>
+  <si>
+    <t>Short Bow</t>
+  </si>
+  <si>
+    <t>Long Bow</t>
+  </si>
+  <si>
+    <t>Crossbow</t>
+  </si>
+  <si>
+    <t>Armor</t>
+  </si>
+  <si>
+    <t>Amulet</t>
+  </si>
+  <si>
+    <t>TestQuestItem</t>
+  </si>
+  <si>
+    <t>Tastes like cereal with a hint of not dying a horible death</t>
+  </si>
+  <si>
+    <t>A key to opportunity, and someone's wallet</t>
+  </si>
+  <si>
+    <t>Chop your foes asunder</t>
+  </si>
+  <si>
+    <t>Big stick with pointy bits, perfect against armor</t>
+  </si>
+  <si>
+    <t>A small nimble blade with many uses</t>
+  </si>
+  <si>
+    <t>Your standard slashing sword</t>
+  </si>
+  <si>
+    <t>A two handed blade with some reach</t>
+  </si>
+  <si>
+    <t>A two handed blade that is comicly big</t>
+  </si>
+  <si>
+    <t>Suprisingly heavy yet faster and more fancy</t>
+  </si>
+  <si>
+    <t>A standard bow. Keep your distance</t>
+  </si>
+  <si>
+    <t>A larger bow meant to hit enemies far away, rather than acros the room</t>
+  </si>
+  <si>
+    <t>Lots of power but needs time to reload</t>
+  </si>
+  <si>
+    <t>Protect thyne knees</t>
+  </si>
+  <si>
+    <t>Feels magical</t>
+  </si>
+  <si>
+    <t>I suppose this is important since I can't drop it</t>
+  </si>
+  <si>
+    <t>Potion_of_Healing</t>
+  </si>
+  <si>
+    <t>Lock_Pick</t>
+  </si>
+  <si>
+    <t>Arming_Sword</t>
+  </si>
+  <si>
+    <t>Long_Sword</t>
+  </si>
+  <si>
+    <t>Great_Sword</t>
+  </si>
+  <si>
+    <t>Short_Bow</t>
+  </si>
+  <si>
+    <t>Long_Bow</t>
+  </si>
+  <si>
+    <t>Test_Quest_Item</t>
+  </si>
+  <si>
+    <t>POTION_OF_HEALING</t>
+  </si>
+  <si>
+    <t>LOCK_PICK</t>
+  </si>
+  <si>
+    <t>AXE</t>
+  </si>
+  <si>
+    <t>MACE</t>
+  </si>
+  <si>
+    <t>DAGGER</t>
+  </si>
+  <si>
+    <t>ARMING_SWORD</t>
+  </si>
+  <si>
+    <t>LONG_SWORD</t>
+  </si>
+  <si>
+    <t>GREAT_SWORD</t>
+  </si>
+  <si>
+    <t>RAPIER</t>
+  </si>
+  <si>
+    <t>SHORT_BOW</t>
+  </si>
+  <si>
+    <t>LONG_BOW</t>
+  </si>
+  <si>
+    <t>CROSSBOW</t>
+  </si>
+  <si>
+    <t>ARMOR</t>
+  </si>
+  <si>
+    <t>AMULET</t>
+  </si>
+  <si>
+    <t>TEST_QEUST_ITEM</t>
+  </si>
+  <si>
+    <t>CONSUMABLE</t>
+  </si>
+  <si>
+    <t>WEAPON</t>
+  </si>
+  <si>
+    <t>QUEST</t>
+  </si>
+  <si>
+    <t>NONE</t>
+  </si>
+  <si>
+    <t>ONE_HAND</t>
+  </si>
+  <si>
+    <t>TWO_HAND</t>
+  </si>
+  <si>
+    <t>ACCESSORY</t>
+  </si>
+  <si>
+    <t>MEDIUM</t>
+  </si>
+  <si>
+    <t>HEAVY</t>
+  </si>
+  <si>
+    <t>VERY_HEAVY</t>
+  </si>
+  <si>
+    <t>VERY_LIGHT</t>
+  </si>
+  <si>
+    <t>SLASHING</t>
+  </si>
+  <si>
+    <t>BLUNT</t>
+  </si>
+  <si>
+    <t>PIERCING</t>
+  </si>
+  <si>
+    <t>CLOSE</t>
+  </si>
+  <si>
+    <t>REACH</t>
+  </si>
+  <si>
+    <t>LONG_REACH</t>
+  </si>
+  <si>
+    <t>RANGED</t>
+  </si>
+  <si>
+    <t>enum(UA)</t>
+  </si>
+  <si>
+    <t>COMMON</t>
+  </si>
+  <si>
+    <t>Attack</t>
   </si>
 </sst>
 </file>
@@ -451,32 +664,32 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:U8"/>
+  <dimension ref="A1:V24"/>
   <sheetViews>
-    <sheetView topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="M7" sqref="M7"/>
+    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
+      <selection activeCell="P10" sqref="P10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="10.5703125" customWidth="1"/>
-    <col min="2" max="2" width="12.28515625" customWidth="1"/>
-    <col min="3" max="3" width="11.42578125" customWidth="1"/>
-    <col min="4" max="4" width="13.42578125" customWidth="1"/>
+    <col min="2" max="2" width="22.5703125" customWidth="1"/>
+    <col min="3" max="3" width="64.42578125" customWidth="1"/>
+    <col min="4" max="4" width="21.28515625" customWidth="1"/>
     <col min="5" max="5" width="12" customWidth="1"/>
-    <col min="6" max="6" width="15" customWidth="1"/>
-    <col min="7" max="7" width="18.42578125" customWidth="1"/>
+    <col min="6" max="6" width="20.28515625" customWidth="1"/>
+    <col min="7" max="7" width="21.5703125" customWidth="1"/>
     <col min="8" max="9" width="19.140625" customWidth="1"/>
     <col min="10" max="10" width="21.28515625" customWidth="1"/>
     <col min="11" max="11" width="15.28515625" customWidth="1"/>
-    <col min="12" max="12" width="11.5703125" customWidth="1"/>
+    <col min="12" max="12" width="16.140625" customWidth="1"/>
     <col min="13" max="13" width="12.5703125" customWidth="1"/>
-    <col min="18" max="18" width="11.140625" customWidth="1"/>
-    <col min="19" max="20" width="10.5703125" customWidth="1"/>
-    <col min="21" max="21" width="12" customWidth="1"/>
+    <col min="19" max="19" width="11.140625" customWidth="1"/>
+    <col min="20" max="21" width="10.5703125" customWidth="1"/>
+    <col min="22" max="22" width="12" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -520,28 +733,31 @@
         <v>13</v>
       </c>
       <c r="O1" t="s">
+        <v>108</v>
+      </c>
+      <c r="P1" t="s">
         <v>14</v>
       </c>
-      <c r="P1" t="s">
+      <c r="Q1" t="s">
         <v>15</v>
       </c>
-      <c r="Q1" t="s">
+      <c r="R1" t="s">
         <v>16</v>
       </c>
-      <c r="R1" t="s">
+      <c r="S1" t="s">
         <v>17</v>
       </c>
-      <c r="S1" t="s">
+      <c r="T1" t="s">
         <v>18</v>
       </c>
-      <c r="T1" t="s">
+      <c r="U1" t="s">
         <v>19</v>
       </c>
-      <c r="U1" t="s">
+      <c r="V1" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="2" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>24</v>
       </c>
@@ -576,7 +792,7 @@
         <v>22</v>
       </c>
       <c r="L2" t="s">
-        <v>22</v>
+        <v>106</v>
       </c>
       <c r="M2" t="s">
         <v>23</v>
@@ -605,22 +821,1046 @@
       <c r="U2" t="s">
         <v>23</v>
       </c>
-    </row>
-    <row r="7" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="V2" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="3" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A3">
+        <v>0</v>
+      </c>
+      <c r="B3" t="s">
+        <v>35</v>
+      </c>
+      <c r="C3" t="s">
+        <v>50</v>
+      </c>
+      <c r="D3" t="s">
+        <v>65</v>
+      </c>
+      <c r="E3">
+        <v>0</v>
+      </c>
+      <c r="F3" t="s">
+        <v>88</v>
+      </c>
+      <c r="G3" t="s">
+        <v>73</v>
+      </c>
+      <c r="H3" t="s">
+        <v>91</v>
+      </c>
+      <c r="I3" t="s">
+        <v>91</v>
+      </c>
+      <c r="J3" t="s">
+        <v>91</v>
+      </c>
+      <c r="K3" t="s">
+        <v>91</v>
+      </c>
+      <c r="L3" t="s">
+        <v>107</v>
+      </c>
+      <c r="M3">
+        <v>0</v>
+      </c>
+      <c r="N3">
+        <v>5</v>
+      </c>
+      <c r="O3">
+        <v>0</v>
+      </c>
+      <c r="P3">
+        <v>0</v>
+      </c>
+      <c r="Q3">
+        <v>0</v>
+      </c>
+      <c r="R3">
+        <v>0</v>
+      </c>
+      <c r="S3">
+        <v>0</v>
+      </c>
+      <c r="T3">
+        <v>1</v>
+      </c>
+      <c r="U3">
+        <v>2</v>
+      </c>
+      <c r="V3">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="4" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A4">
+        <v>0</v>
+      </c>
+      <c r="B4" t="s">
+        <v>36</v>
+      </c>
+      <c r="C4" t="s">
+        <v>51</v>
+      </c>
+      <c r="D4" t="s">
+        <v>66</v>
+      </c>
+      <c r="E4">
+        <v>0</v>
+      </c>
+      <c r="F4" t="s">
+        <v>88</v>
+      </c>
+      <c r="G4" t="s">
+        <v>74</v>
+      </c>
+      <c r="H4" t="s">
+        <v>91</v>
+      </c>
+      <c r="I4" t="s">
+        <v>91</v>
+      </c>
+      <c r="J4" t="s">
+        <v>91</v>
+      </c>
+      <c r="K4" t="s">
+        <v>91</v>
+      </c>
+      <c r="L4" t="s">
+        <v>107</v>
+      </c>
+      <c r="M4">
+        <v>0</v>
+      </c>
+      <c r="N4">
+        <v>0</v>
+      </c>
+      <c r="O4">
+        <v>0</v>
+      </c>
+      <c r="P4">
+        <v>0</v>
+      </c>
+      <c r="Q4">
+        <v>0</v>
+      </c>
+      <c r="R4">
+        <v>5</v>
+      </c>
+      <c r="S4">
+        <v>0</v>
+      </c>
+      <c r="T4">
+        <v>1</v>
+      </c>
+      <c r="U4">
+        <v>2</v>
+      </c>
+      <c r="V4">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="5" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A5">
+        <v>0</v>
+      </c>
+      <c r="B5" t="s">
+        <v>37</v>
+      </c>
+      <c r="C5" t="s">
+        <v>52</v>
+      </c>
+      <c r="D5" t="s">
+        <v>37</v>
+      </c>
+      <c r="E5">
+        <v>0</v>
+      </c>
+      <c r="F5" t="s">
+        <v>89</v>
+      </c>
+      <c r="G5" t="s">
+        <v>75</v>
+      </c>
+      <c r="H5" t="s">
+        <v>92</v>
+      </c>
+      <c r="I5" t="s">
+        <v>95</v>
+      </c>
+      <c r="J5" t="s">
+        <v>99</v>
+      </c>
+      <c r="K5" t="s">
+        <v>95</v>
+      </c>
+      <c r="L5" t="s">
+        <v>107</v>
+      </c>
+      <c r="M5">
+        <v>2</v>
+      </c>
+      <c r="N5">
+        <v>0</v>
+      </c>
+      <c r="O5">
+        <v>2</v>
+      </c>
+      <c r="P5">
+        <v>2</v>
+      </c>
+      <c r="Q5">
+        <v>0</v>
+      </c>
+      <c r="R5">
+        <v>1</v>
+      </c>
+      <c r="S5">
+        <v>2</v>
+      </c>
+      <c r="T5">
+        <v>10</v>
+      </c>
+      <c r="U5">
+        <v>5</v>
+      </c>
+      <c r="V5">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="6" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A6">
+        <v>0</v>
+      </c>
+      <c r="B6" t="s">
+        <v>38</v>
+      </c>
+      <c r="C6" t="s">
+        <v>53</v>
+      </c>
+      <c r="D6" t="s">
+        <v>38</v>
+      </c>
+      <c r="E6">
+        <v>0</v>
+      </c>
+      <c r="F6" t="s">
+        <v>89</v>
+      </c>
+      <c r="G6" t="s">
+        <v>76</v>
+      </c>
+      <c r="H6" t="s">
+        <v>92</v>
+      </c>
+      <c r="I6" t="s">
+        <v>96</v>
+      </c>
+      <c r="J6" t="s">
+        <v>100</v>
+      </c>
+      <c r="K6" t="s">
+        <v>95</v>
+      </c>
+      <c r="L6" t="s">
+        <v>107</v>
+      </c>
+      <c r="M6">
+        <v>3</v>
+      </c>
+      <c r="N6">
+        <v>0</v>
+      </c>
+      <c r="O6">
+        <v>3</v>
+      </c>
+      <c r="P6">
+        <v>3</v>
+      </c>
+      <c r="Q6">
+        <v>0</v>
+      </c>
+      <c r="R6">
+        <v>0</v>
+      </c>
+      <c r="S6">
+        <v>3</v>
+      </c>
+      <c r="T6">
+        <v>10</v>
+      </c>
+      <c r="U6">
+        <v>5</v>
+      </c>
+      <c r="V6">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="7" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A7">
+        <v>0</v>
+      </c>
       <c r="B7" t="s">
+        <v>39</v>
+      </c>
+      <c r="C7" t="s">
+        <v>54</v>
+      </c>
+      <c r="D7" t="s">
+        <v>39</v>
+      </c>
+      <c r="E7">
+        <v>0</v>
+      </c>
+      <c r="F7" t="s">
+        <v>89</v>
+      </c>
+      <c r="G7" t="s">
+        <v>77</v>
+      </c>
+      <c r="H7" t="s">
+        <v>92</v>
+      </c>
+      <c r="I7" t="s">
+        <v>98</v>
+      </c>
+      <c r="J7" t="s">
+        <v>99</v>
+      </c>
+      <c r="K7" t="s">
+        <v>102</v>
+      </c>
+      <c r="L7" t="s">
+        <v>107</v>
+      </c>
+      <c r="M7">
+        <v>1</v>
+      </c>
+      <c r="N7">
+        <v>0</v>
+      </c>
+      <c r="O7">
+        <v>1</v>
+      </c>
+      <c r="P7">
+        <v>1</v>
+      </c>
+      <c r="Q7">
+        <v>0</v>
+      </c>
+      <c r="R7">
+        <v>5</v>
+      </c>
+      <c r="S7">
+        <v>1</v>
+      </c>
+      <c r="T7">
+        <v>10</v>
+      </c>
+      <c r="U7">
+        <v>5</v>
+      </c>
+      <c r="V7">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="8" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A8">
+        <v>0</v>
+      </c>
+      <c r="B8" t="s">
+        <v>40</v>
+      </c>
+      <c r="C8" t="s">
+        <v>55</v>
+      </c>
+      <c r="D8" t="s">
+        <v>67</v>
+      </c>
+      <c r="E8">
+        <v>0</v>
+      </c>
+      <c r="F8" t="s">
+        <v>89</v>
+      </c>
+      <c r="G8" t="s">
+        <v>78</v>
+      </c>
+      <c r="H8" t="s">
+        <v>92</v>
+      </c>
+      <c r="I8" t="s">
+        <v>95</v>
+      </c>
+      <c r="J8" t="s">
+        <v>99</v>
+      </c>
+      <c r="K8" t="s">
+        <v>95</v>
+      </c>
+      <c r="L8" t="s">
+        <v>107</v>
+      </c>
+      <c r="M8">
+        <v>3</v>
+      </c>
+      <c r="N8">
+        <v>0</v>
+      </c>
+      <c r="O8">
+        <v>3</v>
+      </c>
+      <c r="P8">
+        <v>3</v>
+      </c>
+      <c r="Q8">
+        <v>0</v>
+      </c>
+      <c r="R8">
+        <v>1</v>
+      </c>
+      <c r="S8">
+        <v>3</v>
+      </c>
+      <c r="T8">
+        <v>10</v>
+      </c>
+      <c r="U8">
+        <v>5</v>
+      </c>
+      <c r="V8">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="9" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A9">
+        <v>0</v>
+      </c>
+      <c r="B9" t="s">
+        <v>42</v>
+      </c>
+      <c r="C9" t="s">
+        <v>56</v>
+      </c>
+      <c r="D9" t="s">
+        <v>68</v>
+      </c>
+      <c r="E9">
+        <v>0</v>
+      </c>
+      <c r="F9" t="s">
+        <v>89</v>
+      </c>
+      <c r="G9" t="s">
+        <v>79</v>
+      </c>
+      <c r="H9" t="s">
+        <v>93</v>
+      </c>
+      <c r="I9" t="s">
+        <v>96</v>
+      </c>
+      <c r="J9" t="s">
+        <v>99</v>
+      </c>
+      <c r="K9" t="s">
+        <v>103</v>
+      </c>
+      <c r="L9" t="s">
+        <v>107</v>
+      </c>
+      <c r="M9">
+        <v>4</v>
+      </c>
+      <c r="N9">
+        <v>0</v>
+      </c>
+      <c r="O9">
+        <v>4</v>
+      </c>
+      <c r="P9">
+        <v>4</v>
+      </c>
+      <c r="Q9">
+        <v>0</v>
+      </c>
+      <c r="R9">
+        <v>0</v>
+      </c>
+      <c r="S9">
+        <v>4</v>
+      </c>
+      <c r="T9">
+        <v>10</v>
+      </c>
+      <c r="U9">
+        <v>5</v>
+      </c>
+      <c r="V9">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="10" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A10">
+        <v>0</v>
+      </c>
+      <c r="B10" t="s">
+        <v>41</v>
+      </c>
+      <c r="C10" t="s">
+        <v>57</v>
+      </c>
+      <c r="D10" t="s">
+        <v>69</v>
+      </c>
+      <c r="E10">
+        <v>0</v>
+      </c>
+      <c r="F10" t="s">
+        <v>89</v>
+      </c>
+      <c r="G10" t="s">
+        <v>80</v>
+      </c>
+      <c r="H10" t="s">
+        <v>93</v>
+      </c>
+      <c r="I10" t="s">
+        <v>97</v>
+      </c>
+      <c r="J10" t="s">
+        <v>99</v>
+      </c>
+      <c r="K10" t="s">
+        <v>104</v>
+      </c>
+      <c r="L10" t="s">
+        <v>107</v>
+      </c>
+      <c r="M10">
+        <v>6</v>
+      </c>
+      <c r="N10">
+        <v>0</v>
+      </c>
+      <c r="O10">
+        <v>6</v>
+      </c>
+      <c r="P10">
+        <v>6</v>
+      </c>
+      <c r="Q10">
+        <v>0</v>
+      </c>
+      <c r="R10">
+        <v>0</v>
+      </c>
+      <c r="S10">
+        <v>5</v>
+      </c>
+      <c r="T10">
+        <v>10</v>
+      </c>
+      <c r="U10">
+        <v>5</v>
+      </c>
+      <c r="V10">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="11" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A11">
+        <v>0</v>
+      </c>
+      <c r="B11" t="s">
+        <v>43</v>
+      </c>
+      <c r="C11" t="s">
+        <v>58</v>
+      </c>
+      <c r="D11" t="s">
+        <v>43</v>
+      </c>
+      <c r="E11">
+        <v>0</v>
+      </c>
+      <c r="F11" t="s">
+        <v>89</v>
+      </c>
+      <c r="G11" t="s">
+        <v>81</v>
+      </c>
+      <c r="H11" t="s">
+        <v>92</v>
+      </c>
+      <c r="I11" t="s">
+        <v>95</v>
+      </c>
+      <c r="J11" t="s">
+        <v>101</v>
+      </c>
+      <c r="K11" t="s">
+        <v>103</v>
+      </c>
+      <c r="L11" t="s">
+        <v>107</v>
+      </c>
+      <c r="M11">
+        <v>3</v>
+      </c>
+      <c r="N11">
+        <v>0</v>
+      </c>
+      <c r="O11">
+        <v>2</v>
+      </c>
+      <c r="P11">
+        <v>2</v>
+      </c>
+      <c r="Q11">
+        <v>0</v>
+      </c>
+      <c r="R11">
+        <v>2</v>
+      </c>
+      <c r="S11">
+        <v>3</v>
+      </c>
+      <c r="T11">
+        <v>10</v>
+      </c>
+      <c r="U11">
+        <v>5</v>
+      </c>
+      <c r="V11">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="12" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A12">
+        <v>0</v>
+      </c>
+      <c r="B12" t="s">
+        <v>44</v>
+      </c>
+      <c r="C12" t="s">
+        <v>59</v>
+      </c>
+      <c r="D12" t="s">
+        <v>70</v>
+      </c>
+      <c r="E12">
+        <v>0</v>
+      </c>
+      <c r="F12" t="s">
+        <v>89</v>
+      </c>
+      <c r="G12" t="s">
+        <v>82</v>
+      </c>
+      <c r="H12" t="s">
+        <v>93</v>
+      </c>
+      <c r="I12" t="s">
+        <v>95</v>
+      </c>
+      <c r="J12" t="s">
+        <v>101</v>
+      </c>
+      <c r="K12" t="s">
+        <v>105</v>
+      </c>
+      <c r="L12" t="s">
+        <v>107</v>
+      </c>
+      <c r="M12">
+        <v>2</v>
+      </c>
+      <c r="N12">
+        <v>0</v>
+      </c>
+      <c r="O12">
+        <v>2</v>
+      </c>
+      <c r="P12">
+        <v>2</v>
+      </c>
+      <c r="Q12">
+        <v>0</v>
+      </c>
+      <c r="R12">
+        <v>4</v>
+      </c>
+      <c r="S12">
+        <v>2</v>
+      </c>
+      <c r="T12">
+        <v>10</v>
+      </c>
+      <c r="U12">
+        <v>5</v>
+      </c>
+      <c r="V12">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="13" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A13">
+        <v>0</v>
+      </c>
+      <c r="B13" t="s">
+        <v>45</v>
+      </c>
+      <c r="C13" t="s">
+        <v>60</v>
+      </c>
+      <c r="D13" t="s">
+        <v>71</v>
+      </c>
+      <c r="E13">
+        <v>0</v>
+      </c>
+      <c r="F13" t="s">
+        <v>89</v>
+      </c>
+      <c r="G13" t="s">
+        <v>83</v>
+      </c>
+      <c r="H13" t="s">
+        <v>93</v>
+      </c>
+      <c r="I13" t="s">
+        <v>96</v>
+      </c>
+      <c r="J13" t="s">
+        <v>101</v>
+      </c>
+      <c r="K13" t="s">
+        <v>105</v>
+      </c>
+      <c r="L13" t="s">
+        <v>107</v>
+      </c>
+      <c r="M13">
+        <v>3</v>
+      </c>
+      <c r="N13">
+        <v>0</v>
+      </c>
+      <c r="O13">
+        <v>3</v>
+      </c>
+      <c r="P13">
+        <v>3</v>
+      </c>
+      <c r="Q13">
+        <v>0</v>
+      </c>
+      <c r="R13">
+        <v>1</v>
+      </c>
+      <c r="S13">
+        <v>3</v>
+      </c>
+      <c r="T13">
+        <v>10</v>
+      </c>
+      <c r="U13">
+        <v>5</v>
+      </c>
+      <c r="V13">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="14" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A14">
+        <v>0</v>
+      </c>
+      <c r="B14" t="s">
+        <v>46</v>
+      </c>
+      <c r="C14" t="s">
+        <v>61</v>
+      </c>
+      <c r="D14" t="s">
+        <v>46</v>
+      </c>
+      <c r="E14">
+        <v>0</v>
+      </c>
+      <c r="F14" t="s">
+        <v>89</v>
+      </c>
+      <c r="G14" t="s">
+        <v>84</v>
+      </c>
+      <c r="H14" t="s">
+        <v>93</v>
+      </c>
+      <c r="I14" t="s">
+        <v>96</v>
+      </c>
+      <c r="J14" t="s">
+        <v>101</v>
+      </c>
+      <c r="K14" t="s">
+        <v>105</v>
+      </c>
+      <c r="L14" t="s">
+        <v>107</v>
+      </c>
+      <c r="M14">
+        <v>3</v>
+      </c>
+      <c r="N14">
+        <v>0</v>
+      </c>
+      <c r="O14">
+        <v>5</v>
+      </c>
+      <c r="P14">
+        <v>5</v>
+      </c>
+      <c r="Q14">
+        <v>0</v>
+      </c>
+      <c r="R14">
+        <v>0</v>
+      </c>
+      <c r="S14">
+        <v>3</v>
+      </c>
+      <c r="T14">
+        <v>10</v>
+      </c>
+      <c r="U14">
+        <v>5</v>
+      </c>
+      <c r="V14">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="15" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A15">
+        <v>0</v>
+      </c>
+      <c r="B15" t="s">
+        <v>47</v>
+      </c>
+      <c r="C15" t="s">
+        <v>62</v>
+      </c>
+      <c r="D15" t="s">
+        <v>47</v>
+      </c>
+      <c r="E15">
+        <v>0</v>
+      </c>
+      <c r="F15" t="s">
+        <v>85</v>
+      </c>
+      <c r="G15" t="s">
+        <v>85</v>
+      </c>
+      <c r="H15" t="s">
+        <v>85</v>
+      </c>
+      <c r="I15" t="s">
+        <v>96</v>
+      </c>
+      <c r="J15" t="s">
+        <v>91</v>
+      </c>
+      <c r="K15" t="s">
+        <v>91</v>
+      </c>
+      <c r="L15" t="s">
+        <v>107</v>
+      </c>
+      <c r="M15">
+        <v>3</v>
+      </c>
+      <c r="N15">
+        <v>3</v>
+      </c>
+      <c r="O15">
+        <v>0</v>
+      </c>
+      <c r="P15">
+        <v>0</v>
+      </c>
+      <c r="Q15">
+        <v>0</v>
+      </c>
+      <c r="R15">
+        <v>0</v>
+      </c>
+      <c r="S15">
+        <v>3</v>
+      </c>
+      <c r="T15">
+        <v>10</v>
+      </c>
+      <c r="U15">
+        <v>5</v>
+      </c>
+      <c r="V15">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="16" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A16">
+        <v>0</v>
+      </c>
+      <c r="B16" t="s">
+        <v>48</v>
+      </c>
+      <c r="C16" t="s">
+        <v>63</v>
+      </c>
+      <c r="D16" t="s">
+        <v>48</v>
+      </c>
+      <c r="E16">
+        <v>0</v>
+      </c>
+      <c r="F16" t="s">
+        <v>86</v>
+      </c>
+      <c r="G16" t="s">
+        <v>86</v>
+      </c>
+      <c r="H16" t="s">
+        <v>94</v>
+      </c>
+      <c r="I16" t="s">
+        <v>91</v>
+      </c>
+      <c r="J16" t="s">
+        <v>91</v>
+      </c>
+      <c r="K16" t="s">
+        <v>91</v>
+      </c>
+      <c r="L16" t="s">
+        <v>107</v>
+      </c>
+      <c r="M16">
+        <v>1</v>
+      </c>
+      <c r="N16">
+        <v>1</v>
+      </c>
+      <c r="O16">
+        <v>0</v>
+      </c>
+      <c r="P16">
+        <v>0</v>
+      </c>
+      <c r="Q16">
+        <v>3</v>
+      </c>
+      <c r="R16">
+        <v>0</v>
+      </c>
+      <c r="S16">
+        <v>1</v>
+      </c>
+      <c r="T16">
+        <v>10</v>
+      </c>
+      <c r="U16">
+        <v>5</v>
+      </c>
+      <c r="V16">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="17" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A17">
+        <v>0</v>
+      </c>
+      <c r="B17" t="s">
+        <v>49</v>
+      </c>
+      <c r="C17" t="s">
+        <v>64</v>
+      </c>
+      <c r="D17" t="s">
+        <v>72</v>
+      </c>
+      <c r="E17">
+        <v>0</v>
+      </c>
+      <c r="F17" t="s">
+        <v>90</v>
+      </c>
+      <c r="G17" t="s">
+        <v>87</v>
+      </c>
+      <c r="H17" t="s">
+        <v>91</v>
+      </c>
+      <c r="I17" t="s">
+        <v>91</v>
+      </c>
+      <c r="J17" t="s">
+        <v>91</v>
+      </c>
+      <c r="K17" t="s">
+        <v>91</v>
+      </c>
+      <c r="L17" t="s">
+        <v>107</v>
+      </c>
+      <c r="M17">
+        <v>0</v>
+      </c>
+      <c r="N17">
+        <v>0</v>
+      </c>
+      <c r="O17">
+        <v>0</v>
+      </c>
+      <c r="P17">
+        <v>0</v>
+      </c>
+      <c r="Q17">
+        <v>0</v>
+      </c>
+      <c r="R17">
+        <v>0</v>
+      </c>
+      <c r="S17">
+        <v>0</v>
+      </c>
+      <c r="T17">
+        <v>0</v>
+      </c>
+      <c r="U17">
+        <v>0</v>
+      </c>
+      <c r="V17">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="23" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="B23" t="s">
         <v>25</v>
       </c>
-      <c r="M7" t="s">
+      <c r="M23" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="8" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="B8" t="s">
+    <row r="24" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="B24" t="s">
         <v>26</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -628,8 +1868,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L11"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D28" sqref="D28"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E19" sqref="E19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -644,13 +1884,13 @@
   <sheetData>
     <row r="1" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>32</v>
+        <v>2</v>
       </c>
       <c r="B1" t="s">
+        <v>6</v>
+      </c>
+      <c r="C1" t="s">
         <v>33</v>
-      </c>
-      <c r="C1" t="s">
-        <v>34</v>
       </c>
       <c r="D1" t="s">
         <v>30</v>
@@ -680,14 +1920,9 @@
         <v>20</v>
       </c>
     </row>
-    <row r="8" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A8" t="s">
-        <v>36</v>
-      </c>
-    </row>
     <row r="9" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
     <row r="10" spans="1:12" x14ac:dyDescent="0.25">
@@ -697,7 +1932,7 @@
     </row>
     <row r="11" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>37</v>
+        <v>32</v>
       </c>
     </row>
   </sheetData>

</xml_diff>